<commit_message>
kalkulation tabelle nur listenvkpreis
</commit_message>
<xml_diff>
--- a/Challenge IV/handelswarenkalkulation_vxxx.xlsx
+++ b/Challenge IV/handelswarenkalkulation_vxxx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e34764e6b10fa3a5/Desktop/Rechnernetze-I_ITECH/Challenge IV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="8_{3444824E-FCE5-42C8-A740-6949C63957CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{448516A9-F3C5-4551-89CF-F4186453CB12}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="8_{3444824E-FCE5-42C8-A740-6949C63957CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C59B2822-57C8-420A-B9D0-0F4B01675945}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="672" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="672" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vorwärtskalkulation" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Differenzkalkulation" sheetId="4" r:id="rId3"/>
     <sheet name="Anwendungshilfe" sheetId="5" r:id="rId4"/>
     <sheet name="Gesamt" sheetId="6" r:id="rId5"/>
+    <sheet name="Präsentation" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="Drittens">Anwendungshilfe!$B$35</definedName>
@@ -899,7 +900,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="138">
   <si>
     <t>Bemerkung / Kommentar</t>
   </si>
@@ -9599,8 +9600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0E1454-62F5-4677-9A74-9AE140F0C5B3}">
   <dimension ref="A1:AX55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="F26" sqref="A1:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10513,4 +10514,413 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85CABD09-E110-4612-A382-C43A88BAD236}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="98.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="110" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="96" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="96" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="113" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="107" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="115">
+        <v>1390.35</v>
+      </c>
+      <c r="C2" s="111">
+        <v>4</v>
+      </c>
+      <c r="D2" s="116">
+        <f>B2*C2</f>
+        <v>5561.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="108" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="117">
+        <v>2049.2600000000002</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3" s="118">
+        <f t="shared" ref="D3:D23" si="0">B3*C3</f>
+        <v>8197.0400000000009</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="108" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="117">
+        <v>577.17999999999995</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" s="118">
+        <f t="shared" si="0"/>
+        <v>2308.7199999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="108" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="117">
+        <v>10170.92</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" s="118">
+        <f t="shared" si="0"/>
+        <v>30512.760000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="108" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="117">
+        <v>3274.35</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6" s="118">
+        <f t="shared" si="0"/>
+        <v>26194.799999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="108" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="117">
+        <v>204.15</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" s="118">
+        <f t="shared" si="0"/>
+        <v>816.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="108" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="117">
+        <v>555.38</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8" s="118">
+        <f t="shared" si="0"/>
+        <v>3332.2799999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="108" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="117">
+        <v>17.53</v>
+      </c>
+      <c r="C9">
+        <v>25</v>
+      </c>
+      <c r="D9" s="118">
+        <f t="shared" si="0"/>
+        <v>438.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="108" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="117">
+        <v>50.08</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10" s="118">
+        <f t="shared" si="0"/>
+        <v>200.32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="109" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="119">
+        <v>67.17</v>
+      </c>
+      <c r="C11" s="112">
+        <v>5</v>
+      </c>
+      <c r="D11" s="120">
+        <f t="shared" si="0"/>
+        <v>335.85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="110" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="127" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="97" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="122">
+        <f>SUM(D2:D11)</f>
+        <v>77898.020000000019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="107" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="115">
+        <v>38.68</v>
+      </c>
+      <c r="C13" s="111">
+        <v>1</v>
+      </c>
+      <c r="D13" s="116">
+        <f t="shared" si="0"/>
+        <v>38.68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="109" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="119">
+        <v>46.92</v>
+      </c>
+      <c r="C14" s="112">
+        <v>2</v>
+      </c>
+      <c r="D14" s="120">
+        <f t="shared" si="0"/>
+        <v>93.84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="110" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="127" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="97" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" s="122">
+        <f>SUM(D12:D14)</f>
+        <v>78030.540000000008</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="107" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="115">
+        <v>239.55</v>
+      </c>
+      <c r="C16" s="111">
+        <v>2</v>
+      </c>
+      <c r="D16" s="116">
+        <f t="shared" si="0"/>
+        <v>479.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="108" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" s="117">
+        <v>436.93</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" s="118">
+        <f t="shared" si="0"/>
+        <v>873.86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="108" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" s="117">
+        <v>210.33</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" s="118">
+        <f t="shared" si="0"/>
+        <v>420.66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="108" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" s="117">
+        <v>28.31</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="118">
+        <f t="shared" si="0"/>
+        <v>56.62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="108" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="117">
+        <v>53.4</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20" s="118">
+        <f t="shared" si="0"/>
+        <v>213.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="108" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21" s="117">
+        <v>793.08</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" s="118">
+        <f t="shared" si="0"/>
+        <v>1586.16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="108" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="117">
+        <v>17.53</v>
+      </c>
+      <c r="C22">
+        <v>11</v>
+      </c>
+      <c r="D22" s="118">
+        <f t="shared" si="0"/>
+        <v>192.83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="109" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" s="117">
+        <v>24278.44</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" s="118">
+        <f t="shared" si="0"/>
+        <v>48556.88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="127" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="97" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" s="122">
+        <f>SUM(D15:D23)</f>
+        <v>130410.25000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="110" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="121">
+        <v>100</v>
+      </c>
+      <c r="C25" s="96">
+        <v>100</v>
+      </c>
+      <c r="D25" s="122">
+        <f>B25*C25</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="110" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" s="127" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="97" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="122">
+        <f>D24+D25</f>
+        <v>140410.25000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Handelskalk überarbeitet und Präsi
</commit_message>
<xml_diff>
--- a/Challenge IV/handelswarenkalkulation_vxxx.xlsx
+++ b/Challenge IV/handelswarenkalkulation_vxxx.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e34764e6b10fa3a5/Desktop/Rechnernetze-I_ITECH/Challenge IV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmarkmann\Documents\I-Tech\pb6\Challenge IV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="8_{3444824E-FCE5-42C8-A740-6949C63957CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C59B2822-57C8-420A-B9D0-0F4B01675945}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4829486-E927-4923-968C-5E92D2B9E7AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="672" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="672" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Vorwärtskalkulation" sheetId="1" r:id="rId1"/>
-    <sheet name="Rückwärtskalkulation" sheetId="3" r:id="rId2"/>
-    <sheet name="Differenzkalkulation" sheetId="4" r:id="rId3"/>
-    <sheet name="Anwendungshilfe" sheetId="5" r:id="rId4"/>
+    <sheet name="Vorwärtskalkulation" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="Rückwärtskalkulation" sheetId="3" state="hidden" r:id="rId2"/>
+    <sheet name="Differenzkalkulation" sheetId="4" state="hidden" r:id="rId3"/>
+    <sheet name="Anwendungshilfe" sheetId="5" state="hidden" r:id="rId4"/>
     <sheet name="Gesamt" sheetId="6" r:id="rId5"/>
     <sheet name="Präsentation" sheetId="7" r:id="rId6"/>
   </sheets>
@@ -900,7 +900,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="140">
   <si>
     <t>Bemerkung / Kommentar</t>
   </si>
@@ -1517,6 +1517,12 @@
   <si>
     <t>max Entfernung Mars zur Erde</t>
   </si>
+  <si>
+    <t>Netto Verkaufspreis</t>
+  </si>
+  <si>
+    <t>Gesamt Netto Verkaufspreis</t>
+  </si>
 </sst>
 </file>
 
@@ -1531,7 +1537,7 @@
     <numFmt numFmtId="169" formatCode="0.0000\ \ "/>
     <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
   </numFmts>
-  <fonts count="43" x14ac:knownFonts="1">
+  <fonts count="44" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -1818,8 +1824,13 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1841,6 +1852,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2058,7 +2075,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -2339,6 +2356,25 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -2348,7 +2384,79 @@
     <cellStyle name="Standard 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Standard 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -5292,8 +5400,25 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A5C574F4-314B-4FA1-926F-937D70201F92}" name="Tabelle1" displayName="Tabelle1" ref="A1:F26" headerRowBorderDxfId="4" tableBorderDxfId="5">
+  <autoFilter ref="A1:F26" xr:uid="{A5C574F4-314B-4FA1-926F-937D70201F92}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{9345E2CB-39AC-4492-98E2-158F17F31EC2}" name="Gerät" totalsRowLabel="Ergebnis" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{5D0E4D16-64AC-4211-9776-4ED1CEAD6D46}" name="Brutto-Listenverkaufspreis"/>
+    <tableColumn id="6" xr3:uid="{9E40429A-2558-4458-AE33-24D3ADE71721}" name="Netto Verkaufspreis">
+      <calculatedColumnFormula>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{F8FAA9FE-C482-48A5-A69A-B66698EE7A64}" name="Anzahl"/>
+    <tableColumn id="7" xr3:uid="{70181320-5993-43B1-8157-29A7EFBC3FC2}" name="Gesamt Netto Verkaufspreis">
+      <calculatedColumnFormula>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{DB4CB2CE-7FD4-4EEA-A20A-C697C56841D7}" name="Gesamt Brutto-Listenverkaufspreis" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1">
+      <calculatedColumnFormula>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5565,7 +5690,7 @@
   </sheetPr>
   <dimension ref="B1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -6225,6 +6350,7 @@
   <pageMargins left="0" right="0" top="0.78740157480314965" bottom="0.78740157480314965" header="0" footer="0.39370078740157483"/>
   <pageSetup paperSize="9" orientation="landscape" cellComments="atEnd" r:id="rId2"/>
   <headerFooter>
+    <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000 - öffentlich | public -&amp;1#_x000D_</oddHeader>
     <oddFooter xml:space="preserve">&amp;L&amp;8ControllerSpielwiese.de / Vorwärtskalkulation&amp;C&amp;8&amp;H Seite &amp;P&amp;R&amp;8 &amp;D / Verfasser </oddFooter>
   </headerFooter>
   <drawing r:id="rId3"/>
@@ -6240,7 +6366,9 @@
   </sheetPr>
   <dimension ref="B1:M41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6917,6 +7045,7 @@
   <pageMargins left="0" right="0" top="0.78740157480314965" bottom="0.78740157480314965" header="0" footer="0.39370078740157483"/>
   <pageSetup paperSize="9" orientation="landscape" cellComments="atEnd" r:id="rId2"/>
   <headerFooter>
+    <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000 - öffentlich | public -&amp;1#_x000D_</oddHeader>
     <oddFooter xml:space="preserve">&amp;L&amp;8ControllerSpielwiese.de / Rückwärtskalkulation&amp;C&amp;8&amp;H Seite &amp;P&amp;R&amp;8 &amp;D / Verfasser </oddFooter>
   </headerFooter>
   <drawing r:id="rId3"/>
@@ -6932,7 +7061,9 @@
   </sheetPr>
   <dimension ref="B1:J41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7542,6 +7673,7 @@
   <pageMargins left="0" right="0" top="0.78740157480314965" bottom="0.78740157480314965" header="0" footer="0.39370078740157483"/>
   <pageSetup paperSize="9" orientation="landscape" cellComments="atEnd" r:id="rId2"/>
   <headerFooter>
+    <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000 - öffentlich | public -&amp;1#_x000D_</oddHeader>
     <oddFooter xml:space="preserve">&amp;L&amp;8ControllerSpielwiese.de / Differenzkalkulation&amp;C&amp;8&amp;H Seite &amp;P&amp;R&amp;8 &amp;D / Verfasser </oddFooter>
   </headerFooter>
   <drawing r:id="rId3"/>
@@ -7555,7 +7687,8 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9590,6 +9723,7 @@
   <pageMargins left="0.31496062992125984" right="0" top="0.39370078740157483" bottom="0.23622047244094491" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="95" orientation="landscape" r:id="rId4"/>
   <headerFooter>
+    <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000 - öffentlich | public -&amp;1#_x000D_</oddHeader>
     <oddFooter>&amp;L&amp;8C by ControllerSpielwiese.de&amp;C&amp;8Seite &amp;P&amp;R&amp;8Verfasser: Joachim Becker</oddFooter>
   </headerFooter>
   <drawing r:id="rId5"/>
@@ -9601,7 +9735,7 @@
   <dimension ref="A1:AX55"/>
   <sheetViews>
     <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="F26" sqref="A1:F26"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10512,415 +10646,657 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000 - öffentlich | public -&amp;1#_x000D_</oddHeader>
+  </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85CABD09-E110-4612-A382-C43A88BAD236}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="98.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="110" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="133" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="96" t="s">
+      <c r="C1" s="112" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="112" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="113" t="s">
+      <c r="E1" s="112" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="135" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="107" t="s">
+      <c r="G1" s="135"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="131" t="s">
         <v>119</v>
       </c>
       <c r="B2" s="115">
         <v>1390.35</v>
       </c>
-      <c r="C2" s="111">
+      <c r="C2" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>1168.3613445378151</v>
+      </c>
+      <c r="D2" s="111">
         <v>4</v>
       </c>
-      <c r="D2" s="116">
-        <f>B2*C2</f>
+      <c r="E2" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>4673.4453781512602</v>
+      </c>
+      <c r="F2" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>5561.4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="108" t="s">
+      <c r="G2" s="134"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="132" t="s">
         <v>118</v>
       </c>
       <c r="B3" s="117">
         <v>2049.2600000000002</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>1722.0672268907565</v>
+      </c>
+      <c r="D3">
         <v>4</v>
       </c>
-      <c r="D3" s="118">
-        <f t="shared" ref="D3:D23" si="0">B3*C3</f>
+      <c r="E3" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>6888.268907563026</v>
+      </c>
+      <c r="F3" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>8197.0400000000009</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="108" t="s">
+      <c r="G3" s="117"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="132" t="s">
         <v>120</v>
       </c>
       <c r="B4" s="117">
         <v>577.17999999999995</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>485.02521008403357</v>
+      </c>
+      <c r="D4">
         <v>4</v>
       </c>
-      <c r="D4" s="118">
-        <f t="shared" si="0"/>
+      <c r="E4" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>1940.1008403361343</v>
+      </c>
+      <c r="F4" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>2308.7199999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="108" t="s">
+      <c r="G4" s="117"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="132" t="s">
         <v>117</v>
       </c>
       <c r="B5" s="117">
         <v>10170.92</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>8546.9915966386561</v>
+      </c>
+      <c r="D5">
         <v>3</v>
       </c>
-      <c r="D5" s="118">
-        <f t="shared" si="0"/>
+      <c r="E5" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>25640.97478991597</v>
+      </c>
+      <c r="F5" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>30512.760000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="108" t="s">
+      <c r="G5" s="117"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="132" t="s">
         <v>112</v>
       </c>
       <c r="B6" s="117">
         <v>3274.35</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>2751.5546218487393</v>
+      </c>
+      <c r="D6">
         <v>8</v>
       </c>
-      <c r="D6" s="118">
-        <f t="shared" si="0"/>
-        <v>26194.799999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="108" t="s">
+      <c r="E6" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>22012.436974789915</v>
+      </c>
+      <c r="F6" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
+        <v>26194.799999999996</v>
+      </c>
+      <c r="G6" s="117"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="132" t="s">
         <v>130</v>
       </c>
       <c r="B7" s="117">
         <v>204.15</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>171.55462184873952</v>
+      </c>
+      <c r="D7">
         <v>4</v>
       </c>
-      <c r="D7" s="118">
-        <f t="shared" si="0"/>
+      <c r="E7" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>686.21848739495806</v>
+      </c>
+      <c r="F7" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>816.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="108" t="s">
+      <c r="G7" s="117"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="132" t="s">
         <v>113</v>
       </c>
       <c r="B8" s="117">
         <v>555.38</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>466.70588235294122</v>
+      </c>
+      <c r="D8">
         <v>6</v>
       </c>
-      <c r="D8" s="118">
-        <f t="shared" si="0"/>
-        <v>3332.2799999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="108" t="s">
+      <c r="E8" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>2800.2352941176473</v>
+      </c>
+      <c r="F8" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
+        <v>3332.28</v>
+      </c>
+      <c r="G8" s="117"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="132" t="s">
         <v>114</v>
       </c>
       <c r="B9" s="117">
         <v>17.53</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>14.731092436974791</v>
+      </c>
+      <c r="D9">
         <v>25</v>
       </c>
-      <c r="D9" s="118">
-        <f t="shared" si="0"/>
+      <c r="E9" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>368.27731092436977</v>
+      </c>
+      <c r="F9" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>438.25</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="108" t="s">
+      <c r="G9" s="117"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="132" t="s">
         <v>115</v>
       </c>
       <c r="B10" s="117">
         <v>50.08</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>42.084033613445378</v>
+      </c>
+      <c r="D10">
         <v>4</v>
       </c>
-      <c r="D10" s="118">
-        <f t="shared" si="0"/>
+      <c r="E10" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>168.33613445378151</v>
+      </c>
+      <c r="F10" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>200.32</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="109" t="s">
+      <c r="G10" s="117"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="133" t="s">
         <v>116</v>
       </c>
       <c r="B11" s="119">
         <v>67.17</v>
       </c>
-      <c r="C11" s="112">
+      <c r="C11" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>56.445378151260506</v>
+      </c>
+      <c r="D11" s="112">
         <v>5</v>
       </c>
-      <c r="D11" s="120">
-        <f t="shared" si="0"/>
-        <v>335.85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="110" t="s">
+      <c r="E11" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>282.22689075630251</v>
+      </c>
+      <c r="F11" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
+        <v>335.84999999999997</v>
+      </c>
+      <c r="G11" s="117"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="136" t="s">
         <v>105</v>
       </c>
-      <c r="B12" s="127" t="s">
+      <c r="B12" s="137" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="97" t="s">
+      <c r="C12" s="137" t="s">
         <v>107</v>
       </c>
-      <c r="D12" s="122">
-        <f>SUM(D2:D11)</f>
+      <c r="D12" s="138" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="137">
+        <f>SUM(E2:E11)</f>
+        <v>65460.521008403382</v>
+      </c>
+      <c r="F12" s="137">
+        <f>SUM(F2:F11)</f>
         <v>77898.020000000019</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="107" t="s">
+      <c r="G12" s="117"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="131" t="s">
         <v>121</v>
       </c>
       <c r="B13" s="115">
         <v>38.68</v>
       </c>
-      <c r="C13" s="111">
+      <c r="C13" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>32.504201680672267</v>
+      </c>
+      <c r="D13" s="111">
         <v>1</v>
       </c>
-      <c r="D13" s="116">
-        <f t="shared" si="0"/>
-        <v>38.68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="109" t="s">
+      <c r="E13" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>32.504201680672267</v>
+      </c>
+      <c r="F13" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
+        <v>38.679999999999993</v>
+      </c>
+      <c r="G13" s="117"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="133" t="s">
         <v>122</v>
       </c>
       <c r="B14" s="119">
         <v>46.92</v>
       </c>
-      <c r="C14" s="112">
+      <c r="C14" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>39.428571428571431</v>
+      </c>
+      <c r="D14" s="112">
         <v>2</v>
       </c>
-      <c r="D14" s="120">
-        <f t="shared" si="0"/>
+      <c r="E14" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>78.857142857142861</v>
+      </c>
+      <c r="F14" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>93.84</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="110" t="s">
+      <c r="G14" s="117"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="136" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="127" t="s">
+      <c r="B15" s="137" t="s">
         <v>107</v>
       </c>
-      <c r="C15" s="97" t="s">
+      <c r="C15" s="137" t="s">
         <v>107</v>
       </c>
-      <c r="D15" s="122">
-        <f>SUM(D12:D14)</f>
-        <v>78030.540000000008</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="107" t="s">
+      <c r="D15" s="138" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="137">
+        <f>SUM(E13:E14)</f>
+        <v>111.36134453781513</v>
+      </c>
+      <c r="F15" s="137">
+        <f>SUM(F13:F14)</f>
+        <v>132.51999999999998</v>
+      </c>
+      <c r="G15" s="117"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="131" t="s">
         <v>123</v>
       </c>
       <c r="B16" s="115">
         <v>239.55</v>
       </c>
-      <c r="C16" s="111">
+      <c r="C16" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>201.30252100840337</v>
+      </c>
+      <c r="D16" s="111">
         <v>2</v>
       </c>
-      <c r="D16" s="116">
-        <f t="shared" si="0"/>
+      <c r="E16" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>402.60504201680675</v>
+      </c>
+      <c r="F16" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>479.1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="108" t="s">
+      <c r="G16" s="117"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="132" t="s">
         <v>126</v>
       </c>
       <c r="B17" s="117">
         <v>436.93</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>367.1680672268908</v>
+      </c>
+      <c r="D17">
         <v>2</v>
       </c>
-      <c r="D17" s="118">
-        <f t="shared" si="0"/>
+      <c r="E17" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>734.3361344537816</v>
+      </c>
+      <c r="F17" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>873.86</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="108" t="s">
+      <c r="G17" s="117"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="132" t="s">
         <v>125</v>
       </c>
       <c r="B18" s="117">
         <v>210.33</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>176.74789915966389</v>
+      </c>
+      <c r="D18">
         <v>2</v>
       </c>
-      <c r="D18" s="118">
-        <f t="shared" si="0"/>
+      <c r="E18" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>353.49579831932778</v>
+      </c>
+      <c r="F18" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>420.66</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="108" t="s">
+      <c r="G18" s="117"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="132" t="s">
         <v>124</v>
       </c>
       <c r="B19" s="117">
         <v>28.31</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>23.789915966386555</v>
+      </c>
+      <c r="D19">
         <v>2</v>
       </c>
-      <c r="D19" s="118">
-        <f t="shared" si="0"/>
+      <c r="E19" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>47.579831932773111</v>
+      </c>
+      <c r="F19" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>56.62</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="108" t="s">
+      <c r="G19" s="117"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="132" t="s">
         <v>128</v>
       </c>
       <c r="B20" s="117">
         <v>53.4</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>44.873949579831937</v>
+      </c>
+      <c r="D20">
         <v>4</v>
       </c>
-      <c r="D20" s="118">
-        <f t="shared" si="0"/>
-        <v>213.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="108" t="s">
+      <c r="E20" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>179.49579831932775</v>
+      </c>
+      <c r="F20" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
+        <v>213.60000000000002</v>
+      </c>
+      <c r="G20" s="117"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="132" t="s">
         <v>127</v>
       </c>
       <c r="B21" s="117">
         <v>793.08</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>666.45378151260513</v>
+      </c>
+      <c r="D21">
         <v>2</v>
       </c>
-      <c r="D21" s="118">
-        <f t="shared" si="0"/>
+      <c r="E21" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>1332.9075630252103</v>
+      </c>
+      <c r="F21" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>1586.16</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="108" t="s">
+      <c r="G21" s="117"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="132" t="s">
         <v>114</v>
       </c>
       <c r="B22" s="117">
         <v>17.53</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>14.731092436974791</v>
+      </c>
+      <c r="D22">
         <v>11</v>
       </c>
-      <c r="D22" s="118">
-        <f t="shared" si="0"/>
+      <c r="E22" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>162.0420168067227</v>
+      </c>
+      <c r="F22" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>192.83</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="109" t="s">
+      <c r="G22" s="117"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="133" t="s">
         <v>129</v>
       </c>
       <c r="B23" s="117">
         <v>24278.44</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>20402.050420168067</v>
+      </c>
+      <c r="D23">
         <v>2</v>
       </c>
-      <c r="D23" s="118">
-        <f t="shared" si="0"/>
+      <c r="E23" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>40804.100840336134</v>
+      </c>
+      <c r="F23" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>48556.88</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="107" t="s">
+      <c r="G23" s="117"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="139" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="127" t="s">
+      <c r="B24" s="137" t="s">
         <v>107</v>
       </c>
-      <c r="C24" s="97" t="s">
+      <c r="C24" s="137" t="s">
         <v>107</v>
       </c>
-      <c r="D24" s="122">
-        <f>SUM(D15:D23)</f>
-        <v>130410.25000000003</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="110" t="s">
+      <c r="D24" s="138" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="137">
+        <f>SUM(E16:E23)</f>
+        <v>44016.563025210082</v>
+      </c>
+      <c r="F24" s="137">
+        <f>SUM(F16:F23)</f>
+        <v>52379.71</v>
+      </c>
+      <c r="G24" s="117"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="113" t="s">
         <v>109</v>
       </c>
       <c r="B25" s="121">
         <v>100</v>
       </c>
-      <c r="C25" s="96">
+      <c r="C25" s="117">
+        <f>Tabelle1[[#This Row],[Brutto-Listenverkaufspreis]]/1.19</f>
+        <v>84.033613445378151</v>
+      </c>
+      <c r="D25" s="96">
         <v>100</v>
       </c>
-      <c r="D25" s="122">
-        <f>B25*C25</f>
+      <c r="E25" s="117">
+        <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
+        <v>8403.361344537816</v>
+      </c>
+      <c r="F25" s="134">
+        <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>10000</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="110" t="s">
+      <c r="G25" s="117"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="139" t="s">
         <v>110</v>
       </c>
-      <c r="B26" s="127" t="s">
+      <c r="B26" s="140" t="s">
         <v>107</v>
       </c>
-      <c r="C26" s="97" t="s">
+      <c r="C26" s="140" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="122">
-        <f>D24+D25</f>
+      <c r="D26" s="141" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="140">
+        <f>SUM(E12,E15,E24,E25)</f>
+        <v>117991.8067226891</v>
+      </c>
+      <c r="F26" s="140">
+        <f>SUM(F12,F15,F24,F25)</f>
         <v>140410.25000000003</v>
       </c>
+      <c r="G26" s="117"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="43" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000 - öffentlich | public -&amp;1#_x000D_</oddHeader>
+  </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
max entfernung mars erde geändert in excel
</commit_message>
<xml_diff>
--- a/Challenge IV/handelswarenkalkulation_vxxx.xlsx
+++ b/Challenge IV/handelswarenkalkulation_vxxx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmarkmann\Documents\I-Tech\pb6\Challenge IV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lipal\IdeaProjects\Rechnernetze-I_ITECH\Challenge IV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EB5F1D-33DF-4C6C-8CED-A6D01B051880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B642CC99-310D-49D1-B64A-23F639F7A86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="672" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="672" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vorwärtskalkulation" sheetId="1" r:id="rId1"/>
@@ -2078,7 +2078,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -2350,8 +2350,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="170" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2390,15 +2388,15 @@
   <dxfs count="7">
     <dxf>
       <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
@@ -5412,7 +5410,7 @@
     <tableColumn id="5" xr3:uid="{37E6AFBF-43C3-4AED-AC5E-DF546F075524}" name="MwSt 19 %" dataDxfId="2">
       <calculatedColumnFormula>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DB4CB2CE-7FD4-4EEA-A20A-C697C56841D7}" name="Gesamt Brutto-Listenverkaufspreis" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1">
+    <tableColumn id="4" xr3:uid="{DB4CB2CE-7FD4-4EEA-A20A-C697C56841D7}" name="Gesamt Brutto-Listenverkaufspreis" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0">
       <calculatedColumnFormula>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5714,10 +5712,10 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="I2" s="140" t="s">
+      <c r="I2" s="138" t="s">
         <v>96</v>
       </c>
-      <c r="J2" s="141"/>
+      <c r="J2" s="139"/>
     </row>
     <row r="3" spans="2:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
@@ -5728,10 +5726,10 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="139">
+      <c r="B4" s="137">
         <v>72727</v>
       </c>
-      <c r="C4" s="139"/>
+      <c r="C4" s="137"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -6390,10 +6388,10 @@
       <c r="E2" s="51"/>
       <c r="F2" s="51"/>
       <c r="G2" s="2"/>
-      <c r="I2" s="140" t="s">
+      <c r="I2" s="138" t="s">
         <v>96</v>
       </c>
-      <c r="J2" s="141"/>
+      <c r="J2" s="139"/>
     </row>
     <row r="3" spans="2:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
@@ -6404,10 +6402,10 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="139">
+      <c r="B4" s="137">
         <v>72727</v>
       </c>
-      <c r="C4" s="139"/>
+      <c r="C4" s="137"/>
       <c r="D4" s="51"/>
       <c r="E4" s="51"/>
       <c r="F4" s="51"/>
@@ -7085,10 +7083,10 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="I2" s="140" t="s">
+      <c r="I2" s="138" t="s">
         <v>96</v>
       </c>
-      <c r="J2" s="141"/>
+      <c r="J2" s="139"/>
     </row>
     <row r="3" spans="2:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
@@ -7099,10 +7097,10 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="139">
+      <c r="B4" s="137">
         <v>72727</v>
       </c>
-      <c r="C4" s="139"/>
+      <c r="C4" s="137"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -9733,8 +9731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0E1454-62F5-4677-9A74-9AE140F0C5B3}">
   <dimension ref="A1:AX55"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10514,15 +10512,15 @@
       </c>
       <c r="D29">
         <f>B31</f>
-        <v>316119931719.62878</v>
+        <v>421119931719.62878</v>
       </c>
       <c r="E29" s="117">
         <f>B29*D29</f>
-        <v>319281131036.82507</v>
+        <v>425331131036.82507</v>
       </c>
       <c r="F29" s="117">
         <f>C29*D29</f>
-        <v>559532279143.74292</v>
+        <v>745382279143.74292</v>
       </c>
       <c r="H29" s="106"/>
     </row>
@@ -10535,7 +10533,7 @@
       </c>
       <c r="B31">
         <f>(B33+(0.25*B32)+B34+(0.25*B35)+B36)*1.05</f>
-        <v>316119931719.62878</v>
+        <v>421119931719.62878</v>
       </c>
       <c r="H31" s="100"/>
     </row>
@@ -10582,7 +10580,7 @@
         <v>137</v>
       </c>
       <c r="B36">
-        <v>301016265000</v>
+        <v>401016265000</v>
       </c>
       <c r="H36" s="100"/>
     </row>
@@ -10656,7 +10654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85CABD09-E110-4612-A382-C43A88BAD236}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -10691,10 +10689,9 @@
       <c r="F1" s="112" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="132" t="s">
+      <c r="G1" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="132"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="128" t="s">
@@ -10714,15 +10711,15 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>4673.4453781512602</v>
       </c>
-      <c r="F2" s="131">
+      <c r="F2" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>887.95462184873941</v>
       </c>
-      <c r="G2" s="131">
+      <c r="G2" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>5561.4</v>
       </c>
-      <c r="H2" s="131"/>
+      <c r="H2" s="117"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="129" t="s">
@@ -10742,11 +10739,11 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>6888.268907563026</v>
       </c>
-      <c r="F3" s="131">
+      <c r="F3" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>1308.7710924369749</v>
       </c>
-      <c r="G3" s="131">
+      <c r="G3" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>8197.0400000000009</v>
       </c>
@@ -10770,11 +10767,11 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>1940.1008403361343</v>
       </c>
-      <c r="F4" s="131">
+      <c r="F4" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>368.6191596638655</v>
       </c>
-      <c r="G4" s="131">
+      <c r="G4" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>2308.7199999999998</v>
       </c>
@@ -10798,11 +10795,11 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>25640.97478991597</v>
       </c>
-      <c r="F5" s="131">
+      <c r="F5" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>4871.7852100840346</v>
       </c>
-      <c r="G5" s="131">
+      <c r="G5" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>30512.760000000002</v>
       </c>
@@ -10826,11 +10823,11 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>22012.436974789915</v>
       </c>
-      <c r="F6" s="131">
+      <c r="F6" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>4182.3630252100838</v>
       </c>
-      <c r="G6" s="131">
+      <c r="G6" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>26194.799999999996</v>
       </c>
@@ -10854,11 +10851,11 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>686.21848739495806</v>
       </c>
-      <c r="F7" s="131">
+      <c r="F7" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>130.38151260504202</v>
       </c>
-      <c r="G7" s="131">
+      <c r="G7" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>816.6</v>
       </c>
@@ -10882,11 +10879,11 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>2800.2352941176473</v>
       </c>
-      <c r="F8" s="131">
+      <c r="F8" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>532.04470588235301</v>
       </c>
-      <c r="G8" s="131">
+      <c r="G8" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>3332.28</v>
       </c>
@@ -10910,11 +10907,11 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>368.27731092436977</v>
       </c>
-      <c r="F9" s="131">
+      <c r="F9" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>69.972689075630257</v>
       </c>
-      <c r="G9" s="131">
+      <c r="G9" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>438.25</v>
       </c>
@@ -10938,11 +10935,11 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>168.33613445378151</v>
       </c>
-      <c r="F10" s="131">
+      <c r="F10" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>31.983865546218489</v>
       </c>
-      <c r="G10" s="131">
+      <c r="G10" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>200.32</v>
       </c>
@@ -10966,38 +10963,38 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>282.22689075630251</v>
       </c>
-      <c r="F11" s="131">
+      <c r="F11" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>53.623109243697478</v>
       </c>
-      <c r="G11" s="131">
+      <c r="G11" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>335.84999999999997</v>
       </c>
       <c r="H11" s="117"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="133" t="s">
+      <c r="A12" s="131" t="s">
         <v>105</v>
       </c>
-      <c r="B12" s="134" t="s">
+      <c r="B12" s="132" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="134" t="s">
+      <c r="C12" s="132" t="s">
         <v>107</v>
       </c>
-      <c r="D12" s="135" t="s">
+      <c r="D12" s="133" t="s">
         <v>107</v>
       </c>
-      <c r="E12" s="134">
+      <c r="E12" s="132">
         <f>SUM(E2:E11)</f>
         <v>65460.521008403382</v>
       </c>
-      <c r="F12" s="134">
+      <c r="F12" s="132">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>12437.498991596643</v>
       </c>
-      <c r="G12" s="134">
+      <c r="G12" s="132">
         <f>SUM(G2:G11)</f>
         <v>77898.020000000019</v>
       </c>
@@ -11021,11 +11018,11 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>32.504201680672267</v>
       </c>
-      <c r="F13" s="131">
+      <c r="F13" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>6.1757983193277308</v>
       </c>
-      <c r="G13" s="131">
+      <c r="G13" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>38.679999999999993</v>
       </c>
@@ -11049,38 +11046,38 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>78.857142857142861</v>
       </c>
-      <c r="F14" s="131">
+      <c r="F14" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>14.982857142857144</v>
       </c>
-      <c r="G14" s="131">
+      <c r="G14" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>93.84</v>
       </c>
       <c r="H14" s="117"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="133" t="s">
+      <c r="A15" s="131" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="134" t="s">
+      <c r="B15" s="132" t="s">
         <v>107</v>
       </c>
-      <c r="C15" s="134" t="s">
+      <c r="C15" s="132" t="s">
         <v>107</v>
       </c>
-      <c r="D15" s="135" t="s">
+      <c r="D15" s="133" t="s">
         <v>107</v>
       </c>
-      <c r="E15" s="134">
+      <c r="E15" s="132">
         <f>SUM(E13:E14)</f>
         <v>111.36134453781513</v>
       </c>
-      <c r="F15" s="134">
+      <c r="F15" s="132">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>21.158655462184875</v>
       </c>
-      <c r="G15" s="134">
+      <c r="G15" s="132">
         <f>SUM(G13:G14)</f>
         <v>132.51999999999998</v>
       </c>
@@ -11104,11 +11101,11 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>402.60504201680675</v>
       </c>
-      <c r="F16" s="131">
+      <c r="F16" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>76.494957983193288</v>
       </c>
-      <c r="G16" s="131">
+      <c r="G16" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>479.1</v>
       </c>
@@ -11132,11 +11129,11 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>734.3361344537816</v>
       </c>
-      <c r="F17" s="131">
+      <c r="F17" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>139.5238655462185</v>
       </c>
-      <c r="G17" s="131">
+      <c r="G17" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>873.86</v>
       </c>
@@ -11160,11 +11157,11 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>353.49579831932778</v>
       </c>
-      <c r="F18" s="131">
+      <c r="F18" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>67.164201680672278</v>
       </c>
-      <c r="G18" s="131">
+      <c r="G18" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>420.66</v>
       </c>
@@ -11188,11 +11185,11 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>47.579831932773111</v>
       </c>
-      <c r="F19" s="131">
+      <c r="F19" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>9.0401680672268903</v>
       </c>
-      <c r="G19" s="131">
+      <c r="G19" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>56.62</v>
       </c>
@@ -11216,11 +11213,11 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>179.49579831932775</v>
       </c>
-      <c r="F20" s="131">
+      <c r="F20" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>34.104201680672276</v>
       </c>
-      <c r="G20" s="131">
+      <c r="G20" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>213.60000000000002</v>
       </c>
@@ -11244,11 +11241,11 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>1332.9075630252103</v>
       </c>
-      <c r="F21" s="131">
+      <c r="F21" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>253.25243697478996</v>
       </c>
-      <c r="G21" s="131">
+      <c r="G21" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>1586.16</v>
       </c>
@@ -11272,11 +11269,11 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>162.0420168067227</v>
       </c>
-      <c r="F22" s="131">
+      <c r="F22" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>30.787983193277313</v>
       </c>
-      <c r="G22" s="131">
+      <c r="G22" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>192.83</v>
       </c>
@@ -11300,38 +11297,38 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>40804.100840336134</v>
       </c>
-      <c r="F23" s="131">
+      <c r="F23" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>7752.7791596638654</v>
       </c>
-      <c r="G23" s="131">
+      <c r="G23" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>48556.88</v>
       </c>
       <c r="H23" s="117"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="136" t="s">
+      <c r="A24" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="134" t="s">
+      <c r="B24" s="132" t="s">
         <v>107</v>
       </c>
-      <c r="C24" s="134" t="s">
+      <c r="C24" s="132" t="s">
         <v>107</v>
       </c>
-      <c r="D24" s="135" t="s">
+      <c r="D24" s="133" t="s">
         <v>107</v>
       </c>
-      <c r="E24" s="134">
+      <c r="E24" s="132">
         <f>SUM(E16:E23)</f>
         <v>44016.563025210082</v>
       </c>
-      <c r="F24" s="134">
+      <c r="F24" s="132">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>8363.1469747899155</v>
       </c>
-      <c r="G24" s="134">
+      <c r="G24" s="132">
         <f>SUM(G16:G23)</f>
         <v>52379.71</v>
       </c>
@@ -11355,38 +11352,38 @@
         <f>Tabelle1[[#This Row],[Netto Verkaufspreis]]*Tabelle1[[#This Row],[Anzahl]]</f>
         <v>8403.361344537816</v>
       </c>
-      <c r="F25" s="131">
+      <c r="F25" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>1596.6386554621849</v>
       </c>
-      <c r="G25" s="131">
+      <c r="G25" s="117">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*1.19</f>
         <v>10000</v>
       </c>
       <c r="H25" s="117"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="136" t="s">
+      <c r="A26" s="134" t="s">
         <v>110</v>
       </c>
-      <c r="B26" s="137" t="s">
+      <c r="B26" s="135" t="s">
         <v>107</v>
       </c>
-      <c r="C26" s="137" t="s">
+      <c r="C26" s="135" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="138" t="s">
+      <c r="D26" s="136" t="s">
         <v>107</v>
       </c>
-      <c r="E26" s="137">
+      <c r="E26" s="135">
         <f>SUM(E12,E15,E24,E25)</f>
         <v>117991.8067226891</v>
       </c>
-      <c r="F26" s="137">
+      <c r="F26" s="135">
         <f>Tabelle1[[#This Row],[Gesamt Netto Verkaufspreis]]*0.19</f>
         <v>22418.443277310929</v>
       </c>
-      <c r="G26" s="137">
+      <c r="G26" s="135">
         <f>SUM(G12,G15,G24,G25)</f>
         <v>140410.25000000003</v>
       </c>

</xml_diff>